<commit_message>
correction de bug de fonctionnement
</commit_message>
<xml_diff>
--- a/data/processed/2025-03-03.xlsx
+++ b/data/processed/2025-03-03.xlsx
@@ -18,7 +18,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -4483,7 +4483,10 @@
           <t>00:36:47</t>
         </is>
       </c>
-      <c r="B59" s="3" t="inlineStr"/>
+      <c r="B59" s="3">
+        <f>F59/G59</f>
+        <v/>
+      </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>RBEZ8</t>
@@ -4557,7 +4560,10 @@
           <t>00:36:53</t>
         </is>
       </c>
-      <c r="B60" s="3" t="inlineStr"/>
+      <c r="B60" s="3">
+        <f>F60/G60</f>
+        <v/>
+      </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>RBEH5</t>
@@ -4631,7 +4637,10 @@
           <t>06:00:01</t>
         </is>
       </c>
-      <c r="B61" s="3" t="inlineStr"/>
+      <c r="B61" s="3">
+        <f>F61/G61</f>
+        <v/>
+      </c>
       <c r="C61" t="inlineStr">
         <is>
           <t>ZSIH5</t>
@@ -4705,7 +4714,10 @@
           <t>06:00:01</t>
         </is>
       </c>
-      <c r="B62" s="3" t="inlineStr"/>
+      <c r="B62" s="3">
+        <f>F62/G62</f>
+        <v/>
+      </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -4779,7 +4791,10 @@
           <t>06:00:01</t>
         </is>
       </c>
-      <c r="B63" s="3" t="inlineStr"/>
+      <c r="B63" s="3">
+        <f>F63/G63</f>
+        <v/>
+      </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -4853,7 +4868,10 @@
           <t>09:03:19</t>
         </is>
       </c>
-      <c r="B64" s="3" t="inlineStr"/>
+      <c r="B64" s="3">
+        <f>F64/G64</f>
+        <v/>
+      </c>
       <c r="C64" t="inlineStr">
         <is>
           <t>CJEH5</t>
@@ -4927,7 +4945,10 @@
           <t>09:08:29</t>
         </is>
       </c>
-      <c r="B65" s="3" t="inlineStr"/>
+      <c r="B65" s="3">
+        <f>F65/G65</f>
+        <v/>
+      </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>ZTOH5</t>
@@ -5001,7 +5022,10 @@
           <t>09:11:10</t>
         </is>
       </c>
-      <c r="B66" s="3" t="inlineStr"/>
+      <c r="B66" s="3">
+        <f>F66/G66</f>
+        <v/>
+      </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>ZVLH5</t>
@@ -5075,7 +5099,10 @@
           <t>09:11:39</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr"/>
+      <c r="B67" s="3">
+        <f>F67/G67</f>
+        <v/>
+      </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>ZSRH5</t>
@@ -5149,7 +5176,10 @@
           <t>09:12:13</t>
         </is>
       </c>
-      <c r="B68" s="3" t="inlineStr"/>
+      <c r="B68" s="3">
+        <f>F68/G68</f>
+        <v/>
+      </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -5223,7 +5253,10 @@
           <t>09:12:36</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr"/>
+      <c r="B69" s="3">
+        <f>F69/G69</f>
+        <v/>
+      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -5297,7 +5330,10 @@
           <t>09:23:05</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr"/>
+      <c r="B70" s="3">
+        <f>F70/G70</f>
+        <v/>
+      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>ZVLH5</t>
@@ -5371,7 +5407,10 @@
           <t>09:40:38</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr"/>
+      <c r="B71" s="3">
+        <f>F71/G71</f>
+        <v/>
+      </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -5445,7 +5484,10 @@
           <t>09:55:37</t>
         </is>
       </c>
-      <c r="B72" s="3" t="inlineStr"/>
+      <c r="B72" s="3">
+        <f>F72/G72</f>
+        <v/>
+      </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>ZVWH5</t>
@@ -5519,7 +5561,10 @@
           <t>10:07:56</t>
         </is>
       </c>
-      <c r="B73" s="3" t="inlineStr"/>
+      <c r="B73" s="3">
+        <f>F73/G73</f>
+        <v/>
+      </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -5593,7 +5638,10 @@
           <t>10:15:03</t>
         </is>
       </c>
-      <c r="B74" s="3" t="inlineStr"/>
+      <c r="B74" s="3">
+        <f>F74/G74</f>
+        <v/>
+      </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>ZSRH5</t>
@@ -5667,7 +5715,10 @@
           <t>10:56:57</t>
         </is>
       </c>
-      <c r="B75" s="3" t="inlineStr"/>
+      <c r="B75" s="3">
+        <f>F75/G75</f>
+        <v/>
+      </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -5741,7 +5792,10 @@
           <t>11:02:29</t>
         </is>
       </c>
-      <c r="B76" s="3" t="inlineStr"/>
+      <c r="B76" s="3">
+        <f>F76/G76</f>
+        <v/>
+      </c>
       <c r="C76" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -5815,7 +5869,10 @@
           <t>11:07:57</t>
         </is>
       </c>
-      <c r="B77" s="3" t="inlineStr"/>
+      <c r="B77" s="3">
+        <f>F77/G77</f>
+        <v/>
+      </c>
       <c r="C77" t="inlineStr">
         <is>
           <t>ZSRH5</t>
@@ -5889,7 +5946,10 @@
           <t>11:21:02</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr"/>
+      <c r="B78" s="3">
+        <f>F78/G78</f>
+        <v/>
+      </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>ZVLH5</t>
@@ -5963,7 +6023,10 @@
           <t>11:33:20</t>
         </is>
       </c>
-      <c r="B79" s="3" t="inlineStr"/>
+      <c r="B79" s="3">
+        <f>F79/G79</f>
+        <v/>
+      </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>CJEH5</t>
@@ -6037,7 +6100,10 @@
           <t>11:51:15</t>
         </is>
       </c>
-      <c r="B80" s="3" t="inlineStr"/>
+      <c r="B80" s="3">
+        <f>F80/G80</f>
+        <v/>
+      </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -6111,7 +6177,10 @@
           <t>13:50:12</t>
         </is>
       </c>
-      <c r="B81" s="3" t="inlineStr"/>
+      <c r="B81" s="3">
+        <f>F81/G81</f>
+        <v/>
+      </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>ZVLH5</t>
@@ -6185,7 +6254,10 @@
           <t>14:13:38</t>
         </is>
       </c>
-      <c r="B82" s="3" t="inlineStr"/>
+      <c r="B82" s="3">
+        <f>F82/G82</f>
+        <v/>
+      </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -6259,7 +6331,10 @@
           <t>14:17:57</t>
         </is>
       </c>
-      <c r="B83" s="3" t="inlineStr"/>
+      <c r="B83" s="3">
+        <f>F83/G83</f>
+        <v/>
+      </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>ZWOH5</t>
@@ -6333,7 +6408,10 @@
           <t>15:22:02</t>
         </is>
       </c>
-      <c r="B84" s="3" t="inlineStr"/>
+      <c r="B84" s="3">
+        <f>F84/G84</f>
+        <v/>
+      </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -6407,7 +6485,10 @@
           <t>15:30:58</t>
         </is>
       </c>
-      <c r="B85" s="3" t="inlineStr"/>
+      <c r="B85" s="3">
+        <f>F85/G85</f>
+        <v/>
+      </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>ZSIH5</t>
@@ -6481,7 +6562,10 @@
           <t>15:35:36</t>
         </is>
       </c>
-      <c r="B86" s="3" t="inlineStr"/>
+      <c r="B86" s="3">
+        <f>F86/G86</f>
+        <v/>
+      </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -6555,7 +6639,10 @@
           <t>15:38:40</t>
         </is>
       </c>
-      <c r="B87" s="3" t="inlineStr"/>
+      <c r="B87" s="3">
+        <f>F87/G87</f>
+        <v/>
+      </c>
       <c r="C87" t="inlineStr">
         <is>
           <t>ZTYH5</t>
@@ -6629,7 +6716,10 @@
           <t>15:43:13</t>
         </is>
       </c>
-      <c r="B88" s="3" t="inlineStr"/>
+      <c r="B88" s="3">
+        <f>F88/G88</f>
+        <v/>
+      </c>
       <c r="C88" t="inlineStr">
         <is>
           <t>ZTYH5</t>
@@ -6703,7 +6793,10 @@
           <t>15:48:39</t>
         </is>
       </c>
-      <c r="B89" s="3" t="inlineStr"/>
+      <c r="B89" s="3">
+        <f>F89/G89</f>
+        <v/>
+      </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -6777,7 +6870,10 @@
           <t>15:54:34</t>
         </is>
       </c>
-      <c r="B90" s="3" t="inlineStr"/>
+      <c r="B90" s="3">
+        <f>F90/G90</f>
+        <v/>
+      </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -6851,7 +6947,10 @@
           <t>16:09:52</t>
         </is>
       </c>
-      <c r="B91" s="3" t="inlineStr"/>
+      <c r="B91" s="3">
+        <f>F91/G91</f>
+        <v/>
+      </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>ZULH5</t>
@@ -6925,7 +7024,10 @@
           <t>16:16:10</t>
         </is>
       </c>
-      <c r="B92" s="3" t="inlineStr"/>
+      <c r="B92" s="3">
+        <f>F92/G92</f>
+        <v/>
+      </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -6999,7 +7101,10 @@
           <t>16:18:32</t>
         </is>
       </c>
-      <c r="B93" s="3" t="inlineStr"/>
+      <c r="B93" s="3">
+        <f>F93/G93</f>
+        <v/>
+      </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>MURH5</t>
@@ -7073,7 +7178,10 @@
           <t>16:18:47</t>
         </is>
       </c>
-      <c r="B94" s="3" t="inlineStr"/>
+      <c r="B94" s="3">
+        <f>F94/G94</f>
+        <v/>
+      </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>ZTYH5</t>
@@ -7147,7 +7255,10 @@
           <t>16:19:23</t>
         </is>
       </c>
-      <c r="B95" s="3" t="inlineStr"/>
+      <c r="B95" s="3">
+        <f>F95/G95</f>
+        <v/>
+      </c>
       <c r="C95" t="inlineStr">
         <is>
           <t>ZTYH5</t>
@@ -7221,7 +7332,10 @@
           <t>16:28:43</t>
         </is>
       </c>
-      <c r="B96" s="3" t="inlineStr"/>
+      <c r="B96" s="3">
+        <f>F96/G96</f>
+        <v/>
+      </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>ZVLH5</t>
@@ -7295,7 +7409,10 @@
           <t>16:36:11</t>
         </is>
       </c>
-      <c r="B97" s="3" t="inlineStr"/>
+      <c r="B97" s="3">
+        <f>F97/G97</f>
+        <v/>
+      </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>ZSIH5</t>
@@ -7369,7 +7486,10 @@
           <t>16:47:49</t>
         </is>
       </c>
-      <c r="B98" s="3" t="inlineStr"/>
+      <c r="B98" s="3">
+        <f>F98/G98</f>
+        <v/>
+      </c>
       <c r="C98" t="inlineStr">
         <is>
           <t>ZSIH5</t>
@@ -7443,7 +7563,10 @@
           <t>17:10:28</t>
         </is>
       </c>
-      <c r="B99" s="3" t="inlineStr"/>
+      <c r="B99" s="3">
+        <f>F99/G99</f>
+        <v/>
+      </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>ZTWH5</t>
@@ -7517,7 +7640,10 @@
           <t>19:43:15</t>
         </is>
       </c>
-      <c r="B100" s="3" t="inlineStr"/>
+      <c r="B100" s="3">
+        <f>F100/G100</f>
+        <v/>
+      </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>ZTYH5</t>

</xml_diff>